<commit_message>
quiero crear un solo train_test_split para a partir de ahi hacerle a todos y poder graficar mas facil
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -991,22 +991,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4628680854612942</v>
+        <v>0.5810498849275845</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3603959740228815</v>
+        <v>0.610917145371212</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6003298876641755</v>
+        <v>0.7816118892207385</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4188710361812604</v>
+        <v>0.2239904317205436</v>
       </c>
     </row>
   </sheetData>
@@ -1062,22 +1062,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7350670775892014</v>
+        <v>0.6918548791568156</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7878212258727322</v>
+        <v>0.8446574183655695</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8875929392873358</v>
+        <v>0.9190524568084074</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2196529674477486</v>
+        <v>-0.07291511383532523</v>
       </c>
     </row>
   </sheetData>
@@ -1133,22 +1133,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5954445053546944</v>
+        <v>0.6942176303905359</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8330168955623509</v>
+        <v>0.8853505299486987</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9126975926134302</v>
+        <v>0.9409306722329221</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2402945822555412</v>
+        <v>-0.1108380796448769</v>
       </c>
     </row>
   </sheetData>
@@ -1204,22 +1204,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4538677131172378</v>
+        <v>0.4532064780878013</v>
       </c>
       <c r="D2" t="n">
-        <v>0.508338953300392</v>
+        <v>0.440065233326777</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7129789290718149</v>
+        <v>0.6633741277188741</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6342396433954777</v>
+        <v>0.310624504167525</v>
       </c>
     </row>
   </sheetData>
@@ -1275,22 +1275,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6175794785234507</v>
+        <v>0.5118031337185958</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7743973631321944</v>
+        <v>0.5518818102584471</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8799985017783806</v>
+        <v>0.7428874815599245</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2937551742436224</v>
+        <v>0.3075608930465602</v>
       </c>
     </row>
   </sheetData>
@@ -1346,22 +1346,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B2" t="n">
         <v>16</v>
       </c>
-      <c r="B2" t="n">
-        <v>141</v>
-      </c>
       <c r="C2" t="n">
-        <v>0.4121570329235623</v>
+        <v>0.4826264106791714</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5056141283791705</v>
+        <v>1.037497801426076</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7110654881086345</v>
+        <v>1.018576360135103</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3713005986018671</v>
+        <v>-0.6805716499436505</v>
       </c>
     </row>
   </sheetData>
@@ -1417,22 +1417,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5579714008453226</v>
+        <v>0.477622994526035</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5038784557938416</v>
+        <v>0.3783366230554467</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7098439658078679</v>
+        <v>0.6150907437569246</v>
       </c>
       <c r="F2" t="n">
-        <v>0.373458798411112</v>
+        <v>0.3871584094265622</v>
       </c>
     </row>
   </sheetData>
@@ -1488,22 +1488,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7417394081863822</v>
+        <v>0.6247532853511617</v>
       </c>
       <c r="D2" t="n">
-        <v>1.077288484588244</v>
+        <v>0.5509014783289405</v>
       </c>
       <c r="E2" t="n">
-        <v>1.037925086212027</v>
+        <v>0.742227376434567</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1720426223806321</v>
+        <v>-0.02460949500583753</v>
       </c>
     </row>
   </sheetData>
@@ -2571,31 +2571,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5686274509803922</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09998077477632913</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6602434077079107</v>
+        <v>0.4152661064425771</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6384803921568627</v>
+        <v>0.4410427807486632</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8295847750865052</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -2666,31 +2666,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04999038738816457</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0.6764705882352942</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7005347593582888</v>
+        <v>0.6176470588235294</v>
       </c>
       <c r="G2" t="n">
         <v>0.6764705882352942</v>
       </c>
       <c r="H2" t="n">
-        <v>0.666547106647537</v>
+        <v>0.6211636828644501</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8760092272202998</v>
+        <v>0.8300173010380623</v>
       </c>
     </row>
   </sheetData>
@@ -2764,28 +2764,28 @@
         <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5588235294117647</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5588235294117647</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3122837370242215</v>
+        <v>0.6158645276292335</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5588235294117647</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4006659267480577</v>
+        <v>0.461846976552859</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8166089965397924</v>
+        <v>0.7869088811995386</v>
       </c>
     </row>
   </sheetData>
@@ -2844,19 +2844,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5366620114553465</v>
+        <v>0.6013077211281678</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4870547248066529</v>
+        <v>0.5281202066941012</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6978930611538223</v>
+        <v>0.7267187947852327</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1796952182466958</v>
+        <v>-0.3424411177081306</v>
       </c>
     </row>
   </sheetData>
@@ -2912,22 +2912,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3868215117320903</v>
+        <v>0.5506265049906924</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2953342089682264</v>
+        <v>0.4980777357456132</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5434466017634358</v>
+        <v>0.7057462261646272</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2978575147306793</v>
+        <v>-0.2660754574519941</v>
       </c>
     </row>
   </sheetData>
@@ -2983,22 +2983,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4210041135149656</v>
+        <v>0.4954067924349528</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3372007051283548</v>
+        <v>0.5209749223687926</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5806898527857662</v>
+        <v>0.7217859255823659</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1983219893132575</v>
+        <v>-0.3242783521967445</v>
       </c>
     </row>
   </sheetData>
@@ -3057,19 +3057,19 @@
         <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6371500747583697</v>
+        <v>0.7208162461912868</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5827834163807639</v>
+        <v>0.832133534832235</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7634025257888292</v>
+        <v>0.9122135357646448</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06027717482050421</v>
+        <v>-0.05700681345855352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>